<commit_message>
Adjust labour type simulation
- Map adjusted to new codes of model industries
- Code adjusted to new structure of library code
</commit_message>
<xml_diff>
--- a/project_example/Labour_types/data/mapdmod.xlsx
+++ b/project_example/Labour_types/data/mapdmod.xlsx
@@ -196,109 +196,109 @@
     <t>t060</t>
   </si>
   <si>
-    <t>i001</t>
-  </si>
-  <si>
-    <t>i002</t>
-  </si>
-  <si>
-    <t>i003</t>
-  </si>
-  <si>
-    <t>i004</t>
-  </si>
-  <si>
-    <t>i005</t>
-  </si>
-  <si>
-    <t>i006</t>
-  </si>
-  <si>
-    <t>i007</t>
-  </si>
-  <si>
-    <t>i008</t>
-  </si>
-  <si>
-    <t>i009</t>
-  </si>
-  <si>
-    <t>i010</t>
-  </si>
-  <si>
-    <t>i011</t>
-  </si>
-  <si>
-    <t>i012</t>
-  </si>
-  <si>
-    <t>i016</t>
-  </si>
-  <si>
-    <t>i020</t>
-  </si>
-  <si>
-    <t>i021</t>
-  </si>
-  <si>
-    <t>i022</t>
-  </si>
-  <si>
-    <t>i023</t>
-  </si>
-  <si>
-    <t>i024</t>
-  </si>
-  <si>
-    <t>i025</t>
-  </si>
-  <si>
-    <t>i026</t>
-  </si>
-  <si>
-    <t>i027</t>
-  </si>
-  <si>
-    <t>i028</t>
-  </si>
-  <si>
-    <t>i029</t>
-  </si>
-  <si>
-    <t>i030</t>
-  </si>
-  <si>
-    <t>i034</t>
-  </si>
-  <si>
-    <t>i042</t>
-  </si>
-  <si>
-    <t>i045</t>
-  </si>
-  <si>
-    <t>i046</t>
-  </si>
-  <si>
-    <t>i047</t>
-  </si>
-  <si>
-    <t>i048</t>
-  </si>
-  <si>
-    <t>i049</t>
-  </si>
-  <si>
-    <t>i050</t>
-  </si>
-  <si>
-    <t>i056</t>
-  </si>
-  <si>
-    <t>i057</t>
-  </si>
-  <si>
-    <t>i058</t>
+    <t>iPARI</t>
+  </si>
+  <si>
+    <t>iWHEA</t>
+  </si>
+  <si>
+    <t>iOCER</t>
+  </si>
+  <si>
+    <t>iFVEG</t>
+  </si>
+  <si>
+    <t>iOILS</t>
+  </si>
+  <si>
+    <t>iSUGB</t>
+  </si>
+  <si>
+    <t>iFIBR</t>
+  </si>
+  <si>
+    <t>iOTHC</t>
+  </si>
+  <si>
+    <t>iANIM</t>
+  </si>
+  <si>
+    <t>iFORE</t>
+  </si>
+  <si>
+    <t>iFISH</t>
+  </si>
+  <si>
+    <t>iFOSM</t>
+  </si>
+  <si>
+    <t>iOTHM</t>
+  </si>
+  <si>
+    <t>iFBTO</t>
+  </si>
+  <si>
+    <t>iTXWO</t>
+  </si>
+  <si>
+    <t>iCOKE</t>
+  </si>
+  <si>
+    <t>iREFN</t>
+  </si>
+  <si>
+    <t>iCHEM</t>
+  </si>
+  <si>
+    <t>iRUBP</t>
+  </si>
+  <si>
+    <t>iNMMP</t>
+  </si>
+  <si>
+    <t>iMETP</t>
+  </si>
+  <si>
+    <t>iELEC</t>
+  </si>
+  <si>
+    <t>iMACH</t>
+  </si>
+  <si>
+    <t>iELCF</t>
+  </si>
+  <si>
+    <t>iELCG</t>
+  </si>
+  <si>
+    <t>iTRDI</t>
+  </si>
+  <si>
+    <t>iHWAT</t>
+  </si>
+  <si>
+    <t>iWATR</t>
+  </si>
+  <si>
+    <t>iCONS</t>
+  </si>
+  <si>
+    <t>iTRAD</t>
+  </si>
+  <si>
+    <t>iHORE</t>
+  </si>
+  <si>
+    <t>iTRAN</t>
+  </si>
+  <si>
+    <t>iREBA</t>
+  </si>
+  <si>
+    <t>iPUBO</t>
+  </si>
+  <si>
+    <t>iWAST</t>
   </si>
 </sst>
 </file>
@@ -641,10 +641,10 @@
   <dimension ref="A1:AJ61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ61" sqref="AJ61"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>